<commit_message>
feat: choosing columns for quiz, basic error handling/optimization on page reloads, update to README.md, table example update
</commit_message>
<xml_diff>
--- a/tables/all.xlsx
+++ b/tables/all.xlsx
@@ -16,12 +16,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t>m1#MATH</t>
+  </si>
+  <si>
+    <t>q1#QUESTION</t>
+  </si>
+  <si>
+    <t>q2#QUESTION</t>
+  </si>
+  <si>
+    <t>m2#MATH</t>
+  </si>
   <si>
     <t xml:space="preserve">1 + 2 = 3</t>
   </si>
   <si>
+    <t xml:space="preserve">can you read? -&gt; Yes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2+5 = 7</t>
+  </si>
+  <si>
     <t xml:space="preserve">2 / 5 = .4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">who uses the computer? -&gt; me.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 ** 0 = undef</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lim(x-&gt;5, x-5) = 0</t>
   </si>
 </sst>
 </file>
@@ -56,8 +83,11 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -566,10 +596,41 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" ht="14.25">
-      <c r="A2" t="s">
-        <v>1</v>
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25">
+      <c r="D4" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>